<commit_message>
able to upload primers
</commit_message>
<xml_diff>
--- a/api-server/public/primer_template.xlsx
+++ b/api-server/public/primer_template.xlsx
@@ -63,7 +63,7 @@
     <t>Vendor</t>
   </si>
   <si>
-    <t>Other Names
+    <t>tags
 (semicolon-seperated)</t>
   </si>
 </sst>
@@ -227,13 +227,13 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:K1048576" totalsRowShown="0" headerRowDxfId="1" tableBorderDxfId="0">
   <tableColumns count="11">
-    <tableColumn id="1" name="Other Names_x000a_(semicolon-seperated)"/>
     <tableColumn id="11" name="Sequence"/>
     <tableColumn id="2" name="Orientation_x000a_(forward/backward)"/>
     <tableColumn id="3" name="Melting Temperature_x000a_(number only)"/>
     <tableColumn id="4" name="Concentration"/>
     <tableColumn id="10" name="Vendor"/>
     <tableColumn id="5" name="Description or Comment"/>
+    <tableColumn id="1" name="tags_x000a_(semicolon-seperated)"/>
     <tableColumn id="6" name="Date_x000a_(DD/MM/YYYY)"/>
     <tableColumn id="7" name="Plate Barcode"/>
     <tableColumn id="8" name="Well ID"/>
@@ -509,18 +509,18 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="21.54296875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="34.36328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.6328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.54296875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.81640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12" style="1" customWidth="1"/>
-    <col min="7" max="7" width="25.26953125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="34.36328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.54296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.26953125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.54296875" style="1" customWidth="1"/>
     <col min="8" max="8" width="23.1796875" style="1" customWidth="1"/>
     <col min="9" max="9" width="14.1796875" style="1" customWidth="1"/>
     <col min="10" max="10" width="11.54296875" style="1" customWidth="1"/>
@@ -532,25 +532,25 @@
   <sheetData>
     <row r="1" spans="1:11" ht="49.9" customHeight="1">
       <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>0</v>

</xml_diff>